<commit_message>
testing while working on automation process
</commit_message>
<xml_diff>
--- a/UI_report.xlsx
+++ b/UI_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\Documents\Projects\Ruby\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rayni\Documents\Projects\Ruby\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C97A95DB-2069-4070-A42E-5EA150895EB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C86D7FCD-2C51-4EDB-A2D0-BAB72449FFA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5832"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -43,67 +43,43 @@
     <t>Results</t>
   </si>
   <si>
-    <t>&lt;2018-11-11 Sun 17:03&gt;</t>
-  </si>
-  <si>
-    <t>Systems Integrator/VAR</t>
-  </si>
-  <si>
-    <t>90K/yr</t>
-  </si>
-  <si>
-    <t>Mass Hire</t>
-  </si>
-  <si>
-    <t>Janice Quaid jmcquaid@masshiremsw.com</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Follow-up requested answered questions regarding case advisor and last day worked.</t>
-  </si>
-  <si>
-    <t>&lt;2018-11-12 Mon 08:49&gt;</t>
-  </si>
-  <si>
-    <t>IT Support</t>
-  </si>
-  <si>
-    <t>50K/yr</t>
-  </si>
-  <si>
-    <t>Dans PC</t>
-  </si>
-  <si>
-    <t>Dan Adams dan@danpc.net</t>
-  </si>
-  <si>
-    <t>In person</t>
-  </si>
-  <si>
-    <t>Follow-up requested met up at Flat Penny. West St. Berlin</t>
-  </si>
-  <si>
-    <t>Systems Integrator/ VAR</t>
-  </si>
-  <si>
-    <t>$90K</t>
-  </si>
-  <si>
-    <t>MassHire Framingham Career Centers</t>
-  </si>
-  <si>
-    <t>Doug Cole &lt;dcole@masshiremsw.com&gt;</t>
-  </si>
-  <si>
-    <t>Follow-up Requested Fill out BSR packet</t>
-  </si>
-  <si>
-    <t>&lt;2018-11-17 Sat 08:49&gt;</t>
-  </si>
-  <si>
-    <t>Follow-up requested met up at Liberty Tavern. High St. Clinton MA</t>
+    <t>&lt;2018-11-18 Sun 21:56&gt;</t>
+  </si>
+  <si>
+    <t>Systems Integrator VAR</t>
+  </si>
+  <si>
+    <t>$90K/yr</t>
+  </si>
+  <si>
+    <t>http://www.linkedin.com</t>
+  </si>
+  <si>
+    <t>Matthew Handler  - Recruitment Consultant</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>&lt;2018-11-19 Mon 21:56&gt;</t>
+  </si>
+  <si>
+    <t>Sankat Arbat  - Recruiter</t>
+  </si>
+  <si>
+    <t>&lt;2018-11-20 Tue 21:56&gt;</t>
+  </si>
+  <si>
+    <t>Josh Leventhal  - Marketer/Writer</t>
+  </si>
+  <si>
+    <t>&lt;2018-11-21 Wed 21:56&gt;</t>
+  </si>
+  <si>
+    <t>MIRZA ASLAMULLAH BAIG - DBA (Database Administrator)</t>
   </si>
 </sst>
 </file>
@@ -944,14 +920,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1004,65 +978,68 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files for this week
</commit_message>
<xml_diff>
--- a/UI_report.xlsx
+++ b/UI_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rayni\Documents\Projects\Ruby\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C6E1E9-912E-4AFF-984E-AB37088333CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4854942-8A62-447B-B30B-01224B4200CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -43,256 +43,277 @@
     <t>Results</t>
   </si>
   <si>
-    <t>&lt;2019-03-11 Mon 20:15&gt;</t>
-  </si>
-  <si>
-    <t>Business Analyst</t>
+    <t>&lt;2019-03-25 Mon 19:05&gt;</t>
+  </si>
+  <si>
+    <t>SQL Server DBA</t>
+  </si>
+  <si>
+    <t>$90K</t>
+  </si>
+  <si>
+    <t>MassHire Framingham Career Centers</t>
+  </si>
+  <si>
+    <t>Lorraine Pocon lpocon@masshiremsw.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Signed Up for BSR Notifications</t>
+  </si>
+  <si>
+    <t>Ed Lawrence elawrence@masshiremsw.com</t>
+  </si>
+  <si>
+    <t>Confirmation of tomorrows meeting</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-25 Mon 13:50&gt;</t>
+  </si>
+  <si>
+    <t>Oracle E-Business Suite SQA Tester</t>
+  </si>
+  <si>
+    <t>Dimensional Thinking, LLC</t>
+  </si>
+  <si>
+    <t>Amy Borkar via bullhornmail.com</t>
+  </si>
+  <si>
+    <t>Follow up requested</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-25 Mon 16:47&gt;</t>
+  </si>
+  <si>
+    <t>VMware Engineer</t>
+  </si>
+  <si>
+    <t>NTT DATA Services</t>
+  </si>
+  <si>
+    <t>Siddharth Mishra &lt;siddharth.mishra@nttdata.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-25 Mon 17:48&gt;</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
   </si>
   <si>
     <t>Axelon Services Corporation</t>
   </si>
   <si>
-    <t>Tulasi Kaipu &lt;saitulasi.kaipu@axelon.com&gt;</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Follow up requested</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-11 Mon 20:21&gt;</t>
-  </si>
-  <si>
-    <t>Systems &amp; Servers Admin</t>
-  </si>
-  <si>
-    <t>Oxford Global Resources</t>
-  </si>
-  <si>
-    <t>Randi Noonan &lt;randi_noonan@oxfordcorp.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-11 Mon 17:58&gt;</t>
+    <t>Kalyani Munamarthi &lt;kalyani.munamarthi@axelon.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-26 Tue 17:57&gt;</t>
+  </si>
+  <si>
+    <t>MS Access developer</t>
+  </si>
+  <si>
+    <t>ApTask</t>
+  </si>
+  <si>
+    <t>Aravind Vennam &lt;vennam@aptask.com&gt;</t>
+  </si>
+  <si>
+    <t>First follow-up email</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-19 Tue 16:31&gt;</t>
+  </si>
+  <si>
+    <t>Programmer - AllStar Staffing Group - Boston, MA</t>
+  </si>
+  <si>
+    <t>AllStar Staffing Group</t>
+  </si>
+  <si>
+    <t>Rob Greco</t>
+  </si>
+  <si>
+    <t>215-944-8140</t>
+  </si>
+  <si>
+    <t>Talked to Rob and email new resume</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-26 Tue 18:20&gt;</t>
+  </si>
+  <si>
+    <t>DB2 DBA</t>
+  </si>
+  <si>
+    <t>Voto Consulting LLC</t>
+  </si>
+  <si>
+    <t>Himanshu Kumar himanshu@votoconsulting.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-26 Tue 18:26&gt;</t>
+  </si>
+  <si>
+    <t>Help Desk Technical Support</t>
+  </si>
+  <si>
+    <t>http://www.sigmainc.com</t>
+  </si>
+  <si>
+    <t>Surya Ponnada sponnada@sigmainc.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-26 Tue 18:30&gt;</t>
+  </si>
+  <si>
+    <t>Software Developer (2) C#/.net</t>
+  </si>
+  <si>
+    <t>Robert Half Technology</t>
+  </si>
+  <si>
+    <t>Ryan Staab ryan.staab@rht.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-26 Tue 21:56&gt;</t>
+  </si>
+  <si>
+    <t>Systems Integrator VAR</t>
+  </si>
+  <si>
+    <t>$90K/yr</t>
+  </si>
+  <si>
+    <t>http://www.linkedin.com</t>
+  </si>
+  <si>
+    <t>David Talamo Financial MGR</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-27 Wed 19:05&gt;</t>
+  </si>
+  <si>
+    <t>Frank Yeoung</t>
+  </si>
+  <si>
+    <t>Contact maintenance and discussing opportunities</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-27 Wed 20:20&gt;</t>
+  </si>
+  <si>
+    <t>Operations/Project Manager with Salesforce experience</t>
+  </si>
+  <si>
+    <t>US Tech Solutions.</t>
+  </si>
+  <si>
+    <t>Kapil Kumar &lt;kapil@ustechsolutions.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-27 Wed 20:25&gt;</t>
+  </si>
+  <si>
+    <t>Deskside Technician</t>
+  </si>
+  <si>
+    <t>Dipak Domane dipakd@aptask.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-27 Wed 17:58&gt;</t>
   </si>
   <si>
     <t>Systems Integrator</t>
   </si>
   <si>
-    <t>$90K/yr</t>
-  </si>
-  <si>
     <t>Tatnuck Worcester Rd Westboro</t>
   </si>
   <si>
     <t>David Sullivan and Group tatnuck_group@yahoogroups.com</t>
   </si>
   <si>
-    <t>Communicated opportunity to group</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 20:40&gt;</t>
-  </si>
-  <si>
-    <t>Multiple follow-up</t>
-  </si>
-  <si>
-    <t>ZipRecruiter.com</t>
-  </si>
-  <si>
-    <t>Team@ziprecruiter.com</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 20:46&gt;</t>
-  </si>
-  <si>
-    <t>Windows Server Admin</t>
-  </si>
-  <si>
-    <t>KTEK Resourcing</t>
-  </si>
-  <si>
-    <t>Asha Malviya &lt;asha.malviya@ktekresourcing.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 19:05&gt;</t>
-  </si>
-  <si>
-    <t>SQL Server DBA</t>
-  </si>
-  <si>
-    <t>$90K</t>
-  </si>
-  <si>
-    <t>MassHire Framingham Career Centers</t>
-  </si>
-  <si>
-    <t>Ed Lawrence &lt;elawrence@masshiremsw.com&gt;</t>
-  </si>
-  <si>
-    <t>Sent great article on networking</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 20:54&gt;</t>
-  </si>
-  <si>
-    <t>IT Infrastructure Engineer</t>
-  </si>
-  <si>
-    <t>Jelena Stevanovic &lt;Jelena.stevanovic@axelon.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 20:59&gt;</t>
-  </si>
-  <si>
-    <t>Help Desk Operator</t>
-  </si>
-  <si>
-    <t>IT Trailblazers.</t>
-  </si>
-  <si>
-    <t>Dipesh Sahu &lt;dipesh@ittblazers.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 21:05&gt;</t>
-  </si>
-  <si>
-    <t>Java Developer</t>
-  </si>
-  <si>
-    <t>Huxley</t>
-  </si>
-  <si>
-    <t>Michael Draine &lt;m.draine@huxley.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 21:18&gt;</t>
-  </si>
-  <si>
-    <t>Database Administrator</t>
-  </si>
-  <si>
-    <t>Huxley IT</t>
-  </si>
-  <si>
-    <t>Debbie Riva &lt;d.riva@huxley.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 21:27&gt;</t>
-  </si>
-  <si>
-    <t>Desktop Support Technician</t>
-  </si>
-  <si>
-    <t>Robert Half Strategic Accounts</t>
-  </si>
-  <si>
-    <t>Dunn, Brandon (04860) &lt;Brandon.Dunn@roberthalf.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 21:33&gt;</t>
-  </si>
-  <si>
-    <t>Spectraforce Technologies Inc.</t>
-  </si>
-  <si>
-    <t>Diksha &lt;diksha.sharma@spectraforce.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-12 Tue 21:43&gt;</t>
-  </si>
-  <si>
-    <t>Application Engineer</t>
-  </si>
-  <si>
-    <t>Insight Global, LLC</t>
-  </si>
-  <si>
-    <t>Jessie Belz &lt;inmail-hit-reply@linkedin.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-13 Wed 19:05&gt;</t>
-  </si>
-  <si>
-    <t>Frank Yeoung frankxyeung@gmail.com</t>
-  </si>
-  <si>
-    <t>Follow-up on yesterdays meeting events</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-13 Thu 13:14&gt;</t>
-  </si>
-  <si>
-    <t>Onsite Systems Administrator</t>
-  </si>
-  <si>
-    <t>www.matrixonweb.com</t>
-  </si>
-  <si>
-    <t>Rohan Chauhan (Executive Recruiter)</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-14 Thu 19:05&gt;</t>
-  </si>
-  <si>
-    <t>Vic Camilleri vic@vcamilleri.com</t>
-  </si>
-  <si>
-    <t>Provided info on OpenVMS</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-14 Thu 17:58&gt;</t>
-  </si>
-  <si>
-    <t>Emailed new company list I created</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-14 Thu 13:37&gt;</t>
-  </si>
-  <si>
-    <t>QA Automation Engineer</t>
-  </si>
-  <si>
-    <t>www.jvtadvisors.com</t>
-  </si>
-  <si>
-    <t>Brian Jobin &lt;Bjobin@jvtadvisors.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-15 Fri 13:43&gt;</t>
-  </si>
-  <si>
-    <t>Help Desk Support II</t>
-  </si>
-  <si>
-    <t>Matrix Technology Group</t>
-  </si>
-  <si>
-    <t>Vivek Tiwari vtiwari@matrixonweb.com</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-15 Fri 14:05&gt;</t>
-  </si>
-  <si>
-    <t>Python Developer</t>
-  </si>
-  <si>
-    <t>Indotronix International Corporation</t>
-  </si>
-  <si>
-    <t>Tim Mokidi &lt;tim@iic.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;2019-03-16 Sat 17:22&gt;</t>
-  </si>
-  <si>
-    <t>SQA Tester</t>
-  </si>
-  <si>
-    <t>DTG Global Staffing</t>
-  </si>
-  <si>
-    <t>Amy Borkar Amy.Borkar@dtglobalstaffing.com</t>
+    <t>Email reminder of Salesforce event</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-28 Thu 20:51&gt;</t>
+  </si>
+  <si>
+    <t>Web Developer</t>
+  </si>
+  <si>
+    <t>Talent Retriever</t>
+  </si>
+  <si>
+    <t>Leslie Morgan inmail-hit-reply@linkedin.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-28 Thu 21:23&gt;</t>
+  </si>
+  <si>
+    <t>Helpdesk Temp/Perm</t>
+  </si>
+  <si>
+    <t>The CEI Group</t>
+  </si>
+  <si>
+    <t>Daniel DesJardins ddesjardins@theceigroup.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-28 Thu 23:32&gt;</t>
+  </si>
+  <si>
+    <t>Senior Business Data analyst</t>
+  </si>
+  <si>
+    <t>IDC Technologies Inc</t>
+  </si>
+  <si>
+    <t>Ritesh Jaiswal &lt;ritesh.j@idctechnologies.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-29 Fri 07:46&gt;</t>
+  </si>
+  <si>
+    <t>Intermediate Technical Staff</t>
+  </si>
+  <si>
+    <t>ZipRecruiter</t>
+  </si>
+  <si>
+    <t>Phil @ ZipRecruiter &lt;phil@ziprecruiter.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-29 Fri 07:54&gt;</t>
+  </si>
+  <si>
+    <t>PT Evening Instructor</t>
+  </si>
+  <si>
+    <t>MassHire</t>
+  </si>
+  <si>
+    <t>Ed Lawrence elawrence@masshiresw.com</t>
+  </si>
+  <si>
+    <t>&lt;2019-03-30 Sat 19:57&gt;</t>
+  </si>
+  <si>
+    <t>Test Engineer</t>
+  </si>
+  <si>
+    <t>E TalentNetwork</t>
+  </si>
+  <si>
+    <t>Jeremy Williams &lt;jeremyw@etalentnetwork.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1169,143 +1190,143 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1322,10 +1343,10 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1342,10 +1363,10 @@
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1362,10 +1383,10 @@
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1375,226 +1396,226 @@
       <c r="B12" t="s">
         <v>53</v>
       </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
         <v>20</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>